<commit_message>
simplified titles of plots in excel
</commit_message>
<xml_diff>
--- a/excel/example.jpg,example2.jpg.xlsx
+++ b/excel/example.jpg,example2.jpg.xlsx
@@ -304,27 +304,21 @@
   <c:chart>
     <c:title>
       <c:tx>
-        <c:strRef>
-          <c:f>'Plot'!F16</c:f>
-          <c:strCache>
-            <c:ptCount val="1"/>
-            <c:pt idx="0">
-              <c:v>Comparing configurations for droplets of size 0 - 0.15 µm</c:v>
-            </c:pt>
-          </c:strCache>
-        </c:strRef>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing configurations for droplets of size 0 - 0.15 µm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
       </c:tx>
       <c:layout/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -461,27 +455,21 @@
   <c:chart>
     <c:title>
       <c:tx>
-        <c:strRef>
-          <c:f>'Plot'!N16</c:f>
-          <c:strCache>
-            <c:ptCount val="1"/>
-            <c:pt idx="0">
-              <c:v>Comparing configurations for droplets of size 0.15 - 0.6 µm</c:v>
-            </c:pt>
-          </c:strCache>
-        </c:strRef>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing configurations for droplets of size 0.15 - 0.6 µm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
       </c:tx>
       <c:layout/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -618,27 +606,21 @@
   <c:chart>
     <c:title>
       <c:tx>
-        <c:strRef>
-          <c:f>'Plot'!F31</c:f>
-          <c:strCache>
-            <c:ptCount val="1"/>
-            <c:pt idx="0">
-              <c:v>Comparing configurations for droplets of size 0.6 - 2 µm</c:v>
-            </c:pt>
-          </c:strCache>
-        </c:strRef>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing configurations for droplets of size 0.6 - 2 µm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
       </c:tx>
       <c:layout/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -775,27 +757,21 @@
   <c:chart>
     <c:title>
       <c:tx>
-        <c:strRef>
-          <c:f>'Plot'!N31</c:f>
-          <c:strCache>
-            <c:ptCount val="1"/>
-            <c:pt idx="0">
-              <c:v>Comparing configurations for droplets of size &gt;2 µm</c:v>
-            </c:pt>
-          </c:strCache>
-        </c:strRef>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing configurations for droplets of size &gt;2 µm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
       </c:tx>
       <c:layout/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1366,13 +1342,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1386,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0.15</v>
       </c>
@@ -1403,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>0.6</v>
       </c>
@@ -1418,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1433,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:4">
       <c r="B5" t="str">
         <f>"&gt;"&amp;'Plot'!A4&amp;" µm"</f>
         <v>&gt;2 µm</v>
@@ -1443,26 +1419,6 @@
       </c>
       <c r="D5">
         <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="F16" t="str">
-        <f>"Comparing configurations for droplets of size "&amp;B2&amp;""</f>
-        <v>Comparing configurations for droplets of size 0 - 0.15 µm</v>
-      </c>
-      <c r="N16" t="str">
-        <f>"Comparing configurations for droplets of size "&amp;B3&amp;""</f>
-        <v>Comparing configurations for droplets of size 0.15 - 0.6 µm</v>
-      </c>
-    </row>
-    <row r="31" spans="6:14">
-      <c r="F31" t="str">
-        <f>"Comparing configurations for droplets of size "&amp;B4&amp;""</f>
-        <v>Comparing configurations for droplets of size 0.6 - 2 µm</v>
-      </c>
-      <c r="N31" t="str">
-        <f>"Comparing configurations for droplets of size "&amp;B5&amp;""</f>
-        <v>Comparing configurations for droplets of size &gt;2 µm</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code formatting + show average and maximum droplet diameter
</commit_message>
<xml_diff>
--- a/excel/example.jpg,example2.jpg.xlsx
+++ b/excel/example.jpg,example2.jpg.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Droplet diameter [µm] (example.jpg)</t>
   </si>
@@ -34,13 +34,27 @@
   <si>
     <t>example2.jpg</t>
   </si>
+  <si>
+    <t>Average droplet diameter (µm)</t>
+  </si>
+  <si>
+    <t>Maximum droplet diameter (µm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,6 +917,308 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing configurations by average droplet diameter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average droplet diameter (µm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Plot!$C$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>example.jpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>example2.jpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$C$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.320129859006658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6692961301682003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50060001"/>
+        <c:axId val="50060002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50060001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Configuration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50060002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average droplet diameter (µm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing configurations by maximum droplet diameter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plot!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Maximum droplet diameter (µm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Plot!$C$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>example.jpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>example2.jpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plot!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>23.550947379927383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.031078158611825</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50070001"/>
+        <c:axId val="50070002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50070001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Configuration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50070002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50070002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Maximum droplet diameter (µm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50070001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -912,10 +1229,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -938,14 +1255,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -966,16 +1283,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -998,14 +1315,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1026,16 +1343,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1049,6 +1366,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1342,23 +1719,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1419,6 +1796,32 @@
       </c>
       <c r="D5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE('Droplet diameters'!A2:A12)</f>
+        <v>5.320129859006658</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE('Droplet diameters'!B2:B6)</f>
+        <v>3.6692961301682003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>MAX('Droplet diameters'!A2:A12)</f>
+        <v>23.550947379927383</v>
+      </c>
+      <c r="D8">
+        <f>MAX('Droplet diameters'!B2:B6)</f>
+        <v>6.031078158611825</v>
       </c>
     </row>
   </sheetData>
@@ -1436,10 +1839,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added blur step to handle images with noisy background
</commit_message>
<xml_diff>
--- a/excel/example.jpg,example2.jpg.xlsx
+++ b/excel/example.jpg,example2.jpg.xlsx
@@ -979,10 +979,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.320129859006658</c:v>
+                  <c:v>8.315694431335414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6692961301682003</c:v>
+                  <c:v>3.670136931151787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,10 +1130,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23.550947379927383</c:v>
+                  <c:v>23.550652247506846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.031078158611825</c:v>
+                  <c:v>6.030617155121099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1748,7 +1748,7 @@
         <v>0 - 0.15 µm</v>
       </c>
       <c r="C2">
-        <f t="array" ref="C2:C5">frequency('Droplet diameters'!A2:A12,'Plot'!A2:A4)</f>
+        <f t="array" ref="C2:C5">frequency('Droplet diameters'!A2:A8,'Plot'!A2:A4)</f>
         <v>0</v>
       </c>
       <c r="D2">
@@ -1803,12 +1803,12 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f>AVERAGE('Droplet diameters'!A2:A12)</f>
-        <v>5.320129859006658</v>
+        <f>AVERAGE('Droplet diameters'!A2:A8)</f>
+        <v>8.315694431335414</v>
       </c>
       <c r="D7">
         <f>AVERAGE('Droplet diameters'!B2:B6)</f>
-        <v>3.6692961301682003</v>
+        <v>3.670136931151787</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1816,12 +1816,12 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <f>MAX('Droplet diameters'!A2:A12)</f>
-        <v>23.550947379927383</v>
+        <f>MAX('Droplet diameters'!A2:A8)</f>
+        <v>23.550652247506846</v>
       </c>
       <c r="D8">
         <f>MAX('Droplet diameters'!B2:B6)</f>
-        <v>6.031078158611825</v>
+        <v>6.030617155121099</v>
       </c>
     </row>
   </sheetData>
@@ -1832,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1848,15 +1848,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>23.55094737992738</v>
+        <v>23.55065224750685</v>
       </c>
       <c r="B2">
-        <v>6.031078158611825</v>
+        <v>6.030617155121099</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>19.90871253011628</v>
+        <v>19.9056400039448</v>
       </c>
       <c r="B3">
         <v>5.789524626793032</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>10.00026491309117</v>
+        <v>9.996371919901266</v>
       </c>
       <c r="B4">
         <v>4.104663864486439</v>
@@ -1872,15 +1872,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>2.492757603907437</v>
+        <v>2.4392042757347</v>
       </c>
       <c r="B5">
-        <v>2.083590076003744</v>
+        <v>2.088255084412402</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>1.321359854136189</v>
+        <v>1.32030739689701</v>
       </c>
       <c r="B6">
         <v>0.3376239249459611</v>
@@ -1888,32 +1888,12 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.9246211982316703</v>
+        <v>0.9231165248209556</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.1054559969248142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
         <v>0.07456865054232387</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>0.05272799846240712</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>0.05272799846240712</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>0.03728432527116193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>